<commit_message>
Update the mapping of the requirements
</commit_message>
<xml_diff>
--- a/Effort/EffortMassimilianoBonetti.xlsx
+++ b/Effort/EffortMassimilianoBonetti.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/max/Desktop/IS2proj/AbboAccordiBonetti/Effort/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{67E76649-42F3-0843-93F5-44E5706EDB6B}" xr6:coauthVersionLast="41" xr6:coauthVersionMax="41" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CD8201AA-C9B6-3D44-9657-A3D0060447F6}" xr6:coauthVersionLast="41" xr6:coauthVersionMax="41" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="460" windowWidth="28800" windowHeight="16420" xr2:uid="{0B28E5B0-B43E-E940-AC9B-200C96DB78B3}"/>
   </bookViews>
@@ -430,7 +430,7 @@
   <dimension ref="A1:B10"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="150" workbookViewId="0">
-      <selection activeCell="A4" sqref="A4"/>
+      <selection activeCell="B5" sqref="B5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -460,7 +460,7 @@
         <v>1</v>
       </c>
       <c r="B3">
-        <v>1.5</v>
+        <v>2</v>
       </c>
     </row>
     <row r="4" spans="1:2" x14ac:dyDescent="0.2">
@@ -476,7 +476,7 @@
         <v>3</v>
       </c>
       <c r="B5">
-        <v>2</v>
+        <v>3</v>
       </c>
     </row>
     <row r="6" spans="1:2" x14ac:dyDescent="0.2">
@@ -484,7 +484,7 @@
         <v>4</v>
       </c>
       <c r="B6">
-        <v>0.5</v>
+        <v>3</v>
       </c>
     </row>
     <row r="7" spans="1:2" x14ac:dyDescent="0.2">
@@ -497,7 +497,7 @@
         <v>6</v>
       </c>
       <c r="B8">
-        <v>1</v>
+        <v>4</v>
       </c>
     </row>
     <row r="9" spans="1:2" x14ac:dyDescent="0.2">

</xml_diff>

<commit_message>
Add Phenomenon table and Alloy model
</commit_message>
<xml_diff>
--- a/Effort/EffortMassimilianoBonetti.xlsx
+++ b/Effort/EffortMassimilianoBonetti.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/max/Desktop/IS2proj/AbboAccordiBonetti/Effort/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CD8201AA-C9B6-3D44-9657-A3D0060447F6}" xr6:coauthVersionLast="41" xr6:coauthVersionMax="41" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D2BDA742-B768-3D46-8F7F-48CFE6BFC755}" xr6:coauthVersionLast="41" xr6:coauthVersionMax="41" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="460" windowWidth="28800" windowHeight="16420" xr2:uid="{0B28E5B0-B43E-E940-AC9B-200C96DB78B3}"/>
+    <workbookView xWindow="3520" yWindow="460" windowWidth="28800" windowHeight="16340" xr2:uid="{0B28E5B0-B43E-E940-AC9B-200C96DB78B3}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -107,9 +107,10 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="16" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -427,10 +428,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{2283A0BD-A3F0-6040-B65F-FBDAEAD5CFA1}">
-  <dimension ref="A1:B10"/>
+  <dimension ref="A1:E10"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="150" workbookViewId="0">
-      <selection activeCell="B5" sqref="B5"/>
+      <selection activeCell="B3" sqref="B3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -441,73 +442,94 @@
     <col min="4" max="4" width="18.83203125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A1" s="2" t="s">
+    <row r="1" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A1" s="3" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="2"/>
-    </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="B1" s="3"/>
+    </row>
+    <row r="2" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A2" s="1" t="s">
         <v>9</v>
       </c>
       <c r="B2" s="1" t="s">
         <v>10</v>
       </c>
-    </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="D2" s="2">
+        <v>43764</v>
+      </c>
+      <c r="E2" s="2">
+        <v>43765</v>
+      </c>
+    </row>
+    <row r="3" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
         <v>1</v>
       </c>
-      <c r="B3">
+      <c r="C3">
         <v>2</v>
       </c>
     </row>
-    <row r="4" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
         <v>2</v>
       </c>
-      <c r="B4">
+      <c r="C4">
         <v>3</v>
       </c>
-    </row>
-    <row r="5" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="E4">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="5" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
         <v>3</v>
       </c>
-      <c r="B5">
+      <c r="C5">
         <v>3</v>
       </c>
     </row>
-    <row r="6" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A6" t="s">
         <v>4</v>
       </c>
-      <c r="B6">
+      <c r="C6">
         <v>3</v>
       </c>
-    </row>
-    <row r="7" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="D6">
+        <v>0.75</v>
+      </c>
+    </row>
+    <row r="7" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A7" t="s">
         <v>5</v>
       </c>
     </row>
-    <row r="8" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A8" t="s">
         <v>6</v>
       </c>
-      <c r="B8">
+      <c r="C8">
         <v>4</v>
       </c>
-    </row>
-    <row r="9" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="D8">
+        <v>2</v>
+      </c>
+      <c r="E8">
+        <v>0.5</v>
+      </c>
+    </row>
+    <row r="9" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A9" t="s">
         <v>7</v>
       </c>
     </row>
-    <row r="10" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A10" t="s">
         <v>8</v>
+      </c>
+      <c r="E10">
+        <v>2.5</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Update Alloy with facts
</commit_message>
<xml_diff>
--- a/Effort/EffortMassimilianoBonetti.xlsx
+++ b/Effort/EffortMassimilianoBonetti.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/max/Desktop/IS2proj/AbboAccordiBonetti/Effort/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D2BDA742-B768-3D46-8F7F-48CFE6BFC755}" xr6:coauthVersionLast="41" xr6:coauthVersionMax="41" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{750BFF0F-B8C4-094D-90B9-AA87EC9BF08E}" xr6:coauthVersionLast="41" xr6:coauthVersionMax="41" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="3520" yWindow="460" windowWidth="28800" windowHeight="16340" xr2:uid="{0B28E5B0-B43E-E940-AC9B-200C96DB78B3}"/>
+    <workbookView xWindow="0" yWindow="460" windowWidth="28800" windowHeight="16340" xr2:uid="{0B28E5B0-B43E-E940-AC9B-200C96DB78B3}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -107,13 +107,14 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="4">
+  <cellXfs count="5">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="16" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="16" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -428,10 +429,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{2283A0BD-A3F0-6040-B65F-FBDAEAD5CFA1}">
-  <dimension ref="A1:E10"/>
+  <dimension ref="A1:H10"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="150" workbookViewId="0">
-      <selection activeCell="B3" sqref="B3"/>
+      <selection activeCell="H11" sqref="H11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -442,13 +443,13 @@
     <col min="4" max="4" width="18.83203125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A1" s="3" t="s">
         <v>0</v>
       </c>
       <c r="B1" s="3"/>
     </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A2" s="1" t="s">
         <v>9</v>
       </c>
@@ -461,16 +462,28 @@
       <c r="E2" s="2">
         <v>43765</v>
       </c>
-    </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="F2" s="2">
+        <v>43767</v>
+      </c>
+      <c r="G2" s="2">
+        <v>43769</v>
+      </c>
+      <c r="H2" s="4">
+        <v>43770</v>
+      </c>
+    </row>
+    <row r="3" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
         <v>1</v>
       </c>
       <c r="C3">
         <v>2</v>
       </c>
-    </row>
-    <row r="4" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="F3">
+        <v>0.5</v>
+      </c>
+    </row>
+    <row r="4" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
         <v>2</v>
       </c>
@@ -481,7 +494,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="5" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
         <v>3</v>
       </c>
@@ -489,7 +502,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="6" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A6" t="s">
         <v>4</v>
       </c>
@@ -500,12 +513,12 @@
         <v>0.75</v>
       </c>
     </row>
-    <row r="7" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A7" t="s">
         <v>5</v>
       </c>
     </row>
-    <row r="8" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A8" t="s">
         <v>6</v>
       </c>
@@ -518,18 +531,30 @@
       <c r="E8">
         <v>0.5</v>
       </c>
-    </row>
-    <row r="9" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="F8">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="9" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A9" t="s">
         <v>7</v>
       </c>
     </row>
-    <row r="10" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A10" t="s">
         <v>8</v>
       </c>
       <c r="E10">
         <v>2.5</v>
+      </c>
+      <c r="F10">
+        <v>0.5</v>
+      </c>
+      <c r="G10">
+        <v>2</v>
+      </c>
+      <c r="H10">
+        <v>3</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Update alloy with the goals
</commit_message>
<xml_diff>
--- a/Effort/EffortMassimilianoBonetti.xlsx
+++ b/Effort/EffortMassimilianoBonetti.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/max/Desktop/IS2proj/AbboAccordiBonetti/Effort/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{750BFF0F-B8C4-094D-90B9-AA87EC9BF08E}" xr6:coauthVersionLast="41" xr6:coauthVersionMax="41" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{36339A5A-895B-5143-9D7A-DE493C902115}" xr6:coauthVersionLast="41" xr6:coauthVersionMax="41" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="460" windowWidth="28800" windowHeight="16340" xr2:uid="{0B28E5B0-B43E-E940-AC9B-200C96DB78B3}"/>
   </bookViews>
@@ -111,10 +111,10 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="16" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="16" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -444,10 +444,10 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A1" s="3" t="s">
+      <c r="A1" s="4" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="3"/>
+      <c r="B1" s="4"/>
     </row>
     <row r="2" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A2" s="1" t="s">
@@ -468,7 +468,7 @@
       <c r="G2" s="2">
         <v>43769</v>
       </c>
-      <c r="H2" s="4">
+      <c r="H2" s="3">
         <v>43770</v>
       </c>
     </row>
@@ -554,7 +554,7 @@
         <v>2</v>
       </c>
       <c r="H10">
-        <v>3</v>
+        <v>3.5</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Update alloy with the reports and some comments
</commit_message>
<xml_diff>
--- a/Effort/EffortMassimilianoBonetti.xlsx
+++ b/Effort/EffortMassimilianoBonetti.xlsx
@@ -8,14 +8,14 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/max/Desktop/IS2proj/AbboAccordiBonetti/Effort/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{36339A5A-895B-5143-9D7A-DE493C902115}" xr6:coauthVersionLast="41" xr6:coauthVersionMax="41" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{10C032EA-B94F-4C46-BC49-591DAAA91FFF}" xr6:coauthVersionLast="41" xr6:coauthVersionMax="41" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="460" windowWidth="28800" windowHeight="16340" xr2:uid="{0B28E5B0-B43E-E940-AC9B-200C96DB78B3}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="181029"/>
+  <calcPr calcId="191029"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -429,10 +429,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{2283A0BD-A3F0-6040-B65F-FBDAEAD5CFA1}">
-  <dimension ref="A1:H10"/>
+  <dimension ref="A1:J11"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="150" workbookViewId="0">
-      <selection activeCell="H11" sqref="H11"/>
+      <selection activeCell="J10" sqref="J10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -443,13 +443,13 @@
     <col min="4" max="4" width="18.83203125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A1" s="4" t="s">
         <v>0</v>
       </c>
       <c r="B1" s="4"/>
     </row>
-    <row r="2" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A2" s="1" t="s">
         <v>9</v>
       </c>
@@ -472,10 +472,14 @@
         <v>43770</v>
       </c>
     </row>
-    <row r="3" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
         <v>1</v>
       </c>
+      <c r="B3">
+        <f>SUM(C3:S3)</f>
+        <v>2.5</v>
+      </c>
       <c r="C3">
         <v>2</v>
       </c>
@@ -483,10 +487,14 @@
         <v>0.5</v>
       </c>
     </row>
-    <row r="4" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
         <v>2</v>
       </c>
+      <c r="B4">
+        <f t="shared" ref="B4:B10" si="0">SUM(C4:S4)</f>
+        <v>4</v>
+      </c>
       <c r="C4">
         <v>3</v>
       </c>
@@ -494,18 +502,26 @@
         <v>1</v>
       </c>
     </row>
-    <row r="5" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
         <v>3</v>
       </c>
+      <c r="B5">
+        <f t="shared" si="0"/>
+        <v>3</v>
+      </c>
       <c r="C5">
         <v>3</v>
       </c>
     </row>
-    <row r="6" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A6" t="s">
         <v>4</v>
       </c>
+      <c r="B6">
+        <f t="shared" si="0"/>
+        <v>3.75</v>
+      </c>
       <c r="C6">
         <v>3</v>
       </c>
@@ -513,15 +529,26 @@
         <v>0.75</v>
       </c>
     </row>
-    <row r="7" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A7" t="s">
         <v>5</v>
       </c>
-    </row>
-    <row r="8" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="B7">
+        <f t="shared" si="0"/>
+        <v>0.5</v>
+      </c>
+      <c r="I7">
+        <v>0.5</v>
+      </c>
+    </row>
+    <row r="8" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A8" t="s">
         <v>6</v>
       </c>
+      <c r="B8">
+        <f t="shared" si="0"/>
+        <v>7.5</v>
+      </c>
       <c r="C8">
         <v>4</v>
       </c>
@@ -535,15 +562,26 @@
         <v>1</v>
       </c>
     </row>
-    <row r="9" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A9" t="s">
         <v>7</v>
       </c>
-    </row>
-    <row r="10" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="B9">
+        <f t="shared" si="0"/>
+        <v>0.5</v>
+      </c>
+      <c r="I9">
+        <v>0.5</v>
+      </c>
+    </row>
+    <row r="10" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A10" t="s">
         <v>8</v>
       </c>
+      <c r="B10">
+        <f t="shared" si="0"/>
+        <v>13.5</v>
+      </c>
       <c r="E10">
         <v>2.5</v>
       </c>
@@ -554,7 +592,19 @@
         <v>2</v>
       </c>
       <c r="H10">
-        <v>3.5</v>
+        <v>4.5</v>
+      </c>
+      <c r="I10">
+        <v>1</v>
+      </c>
+      <c r="J10">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="11" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="B11">
+        <f>SUM(B3:B10)</f>
+        <v>35.25</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Update the worlds of Alloy with the magic layout
</commit_message>
<xml_diff>
--- a/Effort/EffortMassimilianoBonetti.xlsx
+++ b/Effort/EffortMassimilianoBonetti.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/max/Desktop/IS2proj/AbboAccordiBonetti/Effort/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{10C032EA-B94F-4C46-BC49-591DAAA91FFF}" xr6:coauthVersionLast="41" xr6:coauthVersionMax="41" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E91A9A0E-B274-7540-B626-2A8C85F10F60}" xr6:coauthVersionLast="41" xr6:coauthVersionMax="41" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="460" windowWidth="28800" windowHeight="16340" xr2:uid="{0B28E5B0-B43E-E940-AC9B-200C96DB78B3}"/>
   </bookViews>
@@ -429,10 +429,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{2283A0BD-A3F0-6040-B65F-FBDAEAD5CFA1}">
-  <dimension ref="A1:J11"/>
+  <dimension ref="A1:I10"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="150" workbookViewId="0">
-      <selection activeCell="J10" sqref="J10"/>
+      <selection activeCell="C10" sqref="C10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -443,13 +443,13 @@
     <col min="4" max="4" width="18.83203125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A1" s="4" t="s">
         <v>0</v>
       </c>
       <c r="B1" s="4"/>
     </row>
-    <row r="2" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A2" s="1" t="s">
         <v>9</v>
       </c>
@@ -472,12 +472,11 @@
         <v>43770</v>
       </c>
     </row>
-    <row r="3" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
         <v>1</v>
       </c>
       <c r="B3">
-        <f>SUM(C3:S3)</f>
         <v>2.5</v>
       </c>
       <c r="C3">
@@ -487,12 +486,11 @@
         <v>0.5</v>
       </c>
     </row>
-    <row r="4" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
         <v>2</v>
       </c>
       <c r="B4">
-        <f t="shared" ref="B4:B10" si="0">SUM(C4:S4)</f>
         <v>4</v>
       </c>
       <c r="C4">
@@ -502,25 +500,26 @@
         <v>1</v>
       </c>
     </row>
-    <row r="5" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
         <v>3</v>
       </c>
       <c r="B5">
-        <f t="shared" si="0"/>
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="C5">
         <v>3</v>
       </c>
-    </row>
-    <row r="6" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="I5">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="6" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A6" t="s">
         <v>4</v>
       </c>
       <c r="B6">
-        <f t="shared" si="0"/>
-        <v>3.75</v>
+        <v>4</v>
       </c>
       <c r="C6">
         <v>3</v>
@@ -528,25 +527,26 @@
       <c r="D6">
         <v>0.75</v>
       </c>
-    </row>
-    <row r="7" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="I6">
+        <v>0.25</v>
+      </c>
+    </row>
+    <row r="7" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A7" t="s">
         <v>5</v>
       </c>
       <c r="B7">
-        <f t="shared" si="0"/>
         <v>0.5</v>
       </c>
       <c r="I7">
         <v>0.5</v>
       </c>
     </row>
-    <row r="8" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A8" t="s">
         <v>6</v>
       </c>
       <c r="B8">
-        <f t="shared" si="0"/>
         <v>7.5</v>
       </c>
       <c r="C8">
@@ -562,25 +562,23 @@
         <v>1</v>
       </c>
     </row>
-    <row r="9" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A9" t="s">
         <v>7</v>
       </c>
       <c r="B9">
-        <f t="shared" si="0"/>
         <v>0.5</v>
       </c>
       <c r="I9">
         <v>0.5</v>
       </c>
     </row>
-    <row r="10" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A10" t="s">
         <v>8</v>
       </c>
       <c r="B10">
-        <f t="shared" si="0"/>
-        <v>13.5</v>
+        <v>20.5</v>
       </c>
       <c r="E10">
         <v>2.5</v>
@@ -595,16 +593,7 @@
         <v>4.5</v>
       </c>
       <c r="I10">
-        <v>1</v>
-      </c>
-      <c r="J10">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="11" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="B11">
-        <f>SUM(B3:B10)</f>
-        <v>35.25</v>
+        <v>11</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
update effort of yesterday
</commit_message>
<xml_diff>
--- a/Effort/EffortMassimilianoBonetti.xlsx
+++ b/Effort/EffortMassimilianoBonetti.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="22130"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10211"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Gianmarco Accordi\Documents\Project-INGSW2\AbboAccordiBonetti\Effort\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/max/Desktop/IS2proj/AbboAccordiBonetti/Effort/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B3D52D83-DE02-429D-9DF5-9178334A15EB}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1A9FAA25-EF7A-B04A-95C8-56BD9B4B034D}" xr6:coauthVersionLast="41" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="16440" xr2:uid="{0B28E5B0-B43E-E940-AC9B-200C96DB78B3}"/>
+    <workbookView xWindow="0" yWindow="460" windowWidth="28800" windowHeight="16440" xr2:uid="{0B28E5B0-B43E-E940-AC9B-200C96DB78B3}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -429,171 +429,101 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{2283A0BD-A3F0-6040-B65F-FBDAEAD5CFA1}">
-  <dimension ref="A1:I10"/>
+  <dimension ref="A1:H10"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="150" workbookViewId="0">
-      <selection activeCell="B10" sqref="B3:B10"/>
+      <selection activeCell="D7" sqref="D7"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="11" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="27.625" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="18.625" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="16.875" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="18.875" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="27.6640625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="18.6640625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="16.83203125" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="18.83203125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A1" s="4" t="s">
         <v>0</v>
       </c>
       <c r="B1" s="4"/>
     </row>
-    <row r="2" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A2" s="1" t="s">
         <v>9</v>
       </c>
       <c r="B2" s="1" t="s">
         <v>10</v>
       </c>
-      <c r="D2" s="2">
-        <v>43764</v>
-      </c>
-      <c r="E2" s="2">
-        <v>43765</v>
-      </c>
-      <c r="F2" s="2">
-        <v>43767</v>
-      </c>
-      <c r="G2" s="2">
-        <v>43769</v>
-      </c>
-      <c r="H2" s="3">
-        <v>43770</v>
-      </c>
-    </row>
-    <row r="3" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="D2" s="2"/>
+      <c r="E2" s="2"/>
+      <c r="F2" s="2"/>
+      <c r="G2" s="2"/>
+      <c r="H2" s="3"/>
+    </row>
+    <row r="3" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
         <v>1</v>
       </c>
       <c r="B3">
         <v>2.5</v>
       </c>
-      <c r="C3">
-        <v>2</v>
-      </c>
-      <c r="F3">
-        <v>0.5</v>
-      </c>
-    </row>
-    <row r="4" spans="1:9" x14ac:dyDescent="0.25">
+    </row>
+    <row r="4" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
         <v>2</v>
       </c>
       <c r="B4">
         <v>4</v>
       </c>
-      <c r="C4">
-        <v>3</v>
-      </c>
-      <c r="E4">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="5" spans="1:9" x14ac:dyDescent="0.25">
+    </row>
+    <row r="5" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
         <v>3</v>
       </c>
       <c r="B5">
         <v>4</v>
       </c>
-      <c r="C5">
-        <v>3</v>
-      </c>
-      <c r="I5">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="6" spans="1:9" x14ac:dyDescent="0.25">
+    </row>
+    <row r="6" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A6" t="s">
         <v>4</v>
       </c>
       <c r="B6">
         <v>4</v>
       </c>
-      <c r="C6">
-        <v>3</v>
-      </c>
-      <c r="D6">
-        <v>0.75</v>
-      </c>
-      <c r="I6">
-        <v>0.25</v>
-      </c>
-    </row>
-    <row r="7" spans="1:9" x14ac:dyDescent="0.25">
+    </row>
+    <row r="7" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A7" t="s">
         <v>5</v>
       </c>
       <c r="B7">
-        <v>0.5</v>
-      </c>
-      <c r="I7">
-        <v>0.5</v>
-      </c>
-    </row>
-    <row r="8" spans="1:9" x14ac:dyDescent="0.25">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="8" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A8" t="s">
         <v>6</v>
       </c>
       <c r="B8">
         <v>7.5</v>
       </c>
-      <c r="C8">
-        <v>4</v>
-      </c>
-      <c r="D8">
-        <v>2</v>
-      </c>
-      <c r="E8">
-        <v>0.5</v>
-      </c>
-      <c r="F8">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="9" spans="1:9" x14ac:dyDescent="0.25">
+    </row>
+    <row r="9" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A9" t="s">
         <v>7</v>
       </c>
       <c r="B9">
-        <v>0.5</v>
-      </c>
-      <c r="I9">
-        <v>0.5</v>
-      </c>
-    </row>
-    <row r="10" spans="1:9" x14ac:dyDescent="0.25">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="10" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A10" t="s">
         <v>8</v>
       </c>
       <c r="B10">
-        <v>20.5</v>
-      </c>
-      <c r="E10">
-        <v>2.5</v>
-      </c>
-      <c r="F10">
-        <v>0.5</v>
-      </c>
-      <c r="G10">
-        <v>2</v>
-      </c>
-      <c r="H10">
-        <v>4.5</v>
-      </c>
-      <c r="I10">
-        <v>11</v>
+        <v>18</v>
       </c>
     </row>
   </sheetData>

</xml_diff>